<commit_message>
Added: Functional safety concept for lane assistance item.
</commit_message>
<xml_diff>
--- a/Documents/02_HazardAnalysisAndRiskAssessment_Template.xlsx
+++ b/Documents/02_HazardAnalysisAndRiskAssessment_Template.xlsx
@@ -1581,8 +1581,8 @@
   </sheetPr>
   <dimension ref="A1:AB16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V14" activeCellId="0" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2394,7 +2394,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="44.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.86"/>
@@ -4237,7 +4237,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="84.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.43"/>
@@ -4248,7 +4248,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="38.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="44.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.86"/>
@@ -8854,7 +8854,7 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="51.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="51.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>

</xml_diff>